<commit_message>
mostly done driver b
</commit_message>
<xml_diff>
--- a/694210101R1/LED_switch_pairs.xlsx
+++ b/694210101R1/LED_switch_pairs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\GitHub\Muse\694210101R1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EE6A344-BF7A-4167-87D4-CA8B24E11865}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C67380-7601-4EA8-876B-5CAD833FD9B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7978CB14-2F27-4BCB-813E-6B983813FA6D}"/>
   </bookViews>
@@ -423,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E141B0AC-BBD2-4D99-B106-AE7919EB216F}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1133,7 +1133,7 @@
         <v>102</v>
       </c>
       <c r="D18">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="E18">
         <v>96</v>
@@ -1148,7 +1148,7 @@
         <v>95</v>
       </c>
       <c r="I18">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="J18">
         <v>88</v>
@@ -1235,13 +1235,13 @@
         <v>105</v>
       </c>
       <c r="I20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J20" t="s">
         <v>13</v>
       </c>
       <c r="K20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L20" t="s">
         <v>11</v>

</xml_diff>